<commit_message>
Demodulação funcionando até o 18º bit
</commit_message>
<xml_diff>
--- a/nibble_ascii.xlsx
+++ b/nibble_ascii.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="148">
   <si>
     <t>nibble 1 (bin)</t>
   </si>
@@ -535,13 +535,13 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -831,11 +831,11 @@
       <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>13</v>
+      <c r="K2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="7">
+        <v>1000.0</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>14</v>
@@ -868,18 +868,18 @@
         <f t="shared" si="1"/>
         <v>0.46875</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="8">
         <f t="shared" ref="I3:I18" si="2">IF(EQ(G2,1000),0.5,IF(EQ(G2,(1000+1000/16)),0.5*15/16,IF(EQ(G2,(1000+1000/16*2)),0.5*14/16,IF(EQ(G2,(1000+1000/16*3)),0.5*13/16,IF(EQ(G2,(1000+1000/16*4)),0.5*12/16,IF(EQ(G2,(1000+1000/16*5)),0.5*11/16,IF(EQ(G2,(1000+1000/16*6)),0.5*10/16,IF(EQ(G2,(1000+1000/16*7)),0.5*9/16,IF(EQ(G2,(1000+1000/16*8)),0.5*8/16,IF(EQ(G2,(1000+1000/16*9)),0.5*7/16,IF(EQ(G2,(1000+1000/16*10)),0.5*6/16,IF(EQ(G2,(1000+1000/16*11)),0.5*5/16,IF(EQ(G2,(1000+1000/16*12)),0.5*4/16,IF(EQ(G2,(1000+1000/16*13)),0.5*3/16,IF(EQ(G2,(1000+1000/16*14)),0.5*2/16,IF(EQ(G2,(1000+1000/16*15)),0.5*1/16,IF(EQ(G2,(1000+1000/16*16)),0.5*0/16,0)))))))))))))))))</f>
         <v>0.5</v>
       </c>
       <c r="J3" s="7">
         <v>1000.0</v>
       </c>
-      <c r="K3" s="8">
-        <v>0.5</v>
+      <c r="K3" s="7">
+        <v>0.468</v>
       </c>
       <c r="L3" s="7">
-        <v>1000.0</v>
+        <v>1062.5</v>
       </c>
       <c r="M3" s="1">
         <v>24000.0</v>
@@ -912,7 +912,7 @@
         <f t="shared" si="1"/>
         <v>0.4375</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="8">
         <f t="shared" si="2"/>
         <v>0.46875</v>
       </c>
@@ -921,10 +921,10 @@
         <v>1062.5</v>
       </c>
       <c r="K4" s="7">
-        <v>0.468</v>
+        <v>0.437</v>
       </c>
       <c r="L4" s="7">
-        <v>1062.5</v>
+        <v>1125.0</v>
       </c>
       <c r="M4" s="1">
         <v>22500.0</v>
@@ -957,7 +957,7 @@
         <f t="shared" si="1"/>
         <v>0.40625</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="8">
         <f t="shared" si="2"/>
         <v>0.4375</v>
       </c>
@@ -966,10 +966,10 @@
         <v>1125</v>
       </c>
       <c r="K5" s="7">
-        <v>0.437</v>
+        <v>0.406</v>
       </c>
       <c r="L5" s="7">
-        <v>1125.0</v>
+        <v>1187.5</v>
       </c>
       <c r="M5" s="1">
         <v>21000.0</v>
@@ -1002,7 +1002,7 @@
         <f t="shared" si="1"/>
         <v>0.375</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="8">
         <f t="shared" si="2"/>
         <v>0.40625</v>
       </c>
@@ -1010,11 +1010,11 @@
         <f>1000 + 1000/16*3</f>
         <v>1187.5</v>
       </c>
-      <c r="K6" s="7">
-        <v>0.406</v>
+      <c r="K6" s="8">
+        <v>0.375</v>
       </c>
       <c r="L6" s="7">
-        <v>1187.5</v>
+        <v>1250.0</v>
       </c>
       <c r="M6" s="1">
         <v>19500.0</v>
@@ -1047,7 +1047,7 @@
         <f t="shared" si="1"/>
         <v>0.34375</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="8">
         <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
@@ -1055,11 +1055,11 @@
         <f>1000 + 1000/16*4</f>
         <v>1250</v>
       </c>
-      <c r="K7" s="6">
-        <v>0.375</v>
+      <c r="K7" s="7">
+        <v>0.343</v>
       </c>
       <c r="L7" s="7">
-        <v>1250.0</v>
+        <v>1312.5</v>
       </c>
       <c r="M7" s="1">
         <v>18000.0</v>
@@ -1092,7 +1092,7 @@
         <f t="shared" si="1"/>
         <v>0.3125</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="8">
         <f t="shared" si="2"/>
         <v>0.34375</v>
       </c>
@@ -1101,10 +1101,10 @@
         <v>1312.5</v>
       </c>
       <c r="K8" s="7">
-        <v>0.343</v>
+        <v>0.312</v>
       </c>
       <c r="L8" s="7">
-        <v>1312.5</v>
+        <v>1375.0</v>
       </c>
       <c r="M8" s="1">
         <v>16500.0</v>
@@ -1137,7 +1137,7 @@
         <f t="shared" si="1"/>
         <v>0.28125</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="8">
         <f t="shared" si="2"/>
         <v>0.3125</v>
       </c>
@@ -1146,10 +1146,10 @@
         <v>1375</v>
       </c>
       <c r="K9" s="7">
-        <v>0.312</v>
+        <v>0.281</v>
       </c>
       <c r="L9" s="7">
-        <v>1375.0</v>
+        <v>1437.5</v>
       </c>
       <c r="M9" s="1">
         <v>15000.0</v>
@@ -1182,7 +1182,7 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="8">
         <f t="shared" si="2"/>
         <v>0.28125</v>
       </c>
@@ -1190,11 +1190,11 @@
         <f>1000 + 1000/16*7</f>
         <v>1437.5</v>
       </c>
-      <c r="K10" s="7">
-        <v>0.281</v>
+      <c r="K10" s="6">
+        <v>0.25</v>
       </c>
       <c r="L10" s="7">
-        <v>1437.5</v>
+        <v>1500.0</v>
       </c>
       <c r="M10" s="1">
         <v>13500.0</v>
@@ -1227,7 +1227,7 @@
         <f t="shared" si="1"/>
         <v>0.21875</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="8">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
@@ -1235,11 +1235,11 @@
         <f>1000 + 1000/16*8</f>
         <v>1500</v>
       </c>
-      <c r="K11" s="8">
-        <v>0.25</v>
+      <c r="K11" s="7">
+        <v>0.218</v>
       </c>
       <c r="L11" s="7">
-        <v>1500.0</v>
+        <v>1562.5</v>
       </c>
       <c r="M11" s="1">
         <v>12000.0</v>
@@ -1272,7 +1272,7 @@
         <f t="shared" si="1"/>
         <v>0.1875</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="8">
         <f t="shared" si="2"/>
         <v>0.21875</v>
       </c>
@@ -1281,10 +1281,10 @@
         <v>1562.5</v>
       </c>
       <c r="K12" s="7">
-        <v>0.218</v>
+        <v>0.187</v>
       </c>
       <c r="L12" s="7">
-        <v>1562.5</v>
+        <v>1625.0</v>
       </c>
       <c r="M12" s="1">
         <v>10500.0</v>
@@ -1317,7 +1317,7 @@
         <f t="shared" si="1"/>
         <v>0.15625</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="8">
         <f t="shared" si="2"/>
         <v>0.1875</v>
       </c>
@@ -1326,10 +1326,10 @@
         <v>1625</v>
       </c>
       <c r="K13" s="7">
-        <v>0.187</v>
+        <v>0.156</v>
       </c>
       <c r="L13" s="7">
-        <v>1625.0</v>
+        <v>1687.5</v>
       </c>
       <c r="M13" s="1">
         <v>9000.0</v>
@@ -1362,7 +1362,7 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="8">
         <f t="shared" si="2"/>
         <v>0.15625</v>
       </c>
@@ -1370,11 +1370,11 @@
         <f>1000 + 1000/16*11</f>
         <v>1687.5</v>
       </c>
-      <c r="K14" s="7">
-        <v>0.156</v>
+      <c r="K14" s="8">
+        <v>0.125</v>
       </c>
       <c r="L14" s="7">
-        <v>1687.5</v>
+        <v>1750.0</v>
       </c>
       <c r="M14" s="1">
         <v>7500.0</v>
@@ -1407,7 +1407,7 @@
         <f t="shared" si="1"/>
         <v>0.09375</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="8">
         <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
@@ -1415,11 +1415,11 @@
         <f>1000 + 1000/16*12</f>
         <v>1750</v>
       </c>
-      <c r="K15" s="6">
-        <v>0.125</v>
+      <c r="K15" s="7">
+        <v>0.093</v>
       </c>
       <c r="L15" s="7">
-        <v>1750.0</v>
+        <v>1812.5</v>
       </c>
       <c r="M15" s="1">
         <v>6000.0</v>
@@ -1452,7 +1452,7 @@
         <f t="shared" si="1"/>
         <v>0.0625</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="8">
         <f t="shared" si="2"/>
         <v>0.09375</v>
       </c>
@@ -1461,10 +1461,10 @@
         <v>1812.5</v>
       </c>
       <c r="K16" s="7">
-        <v>0.093</v>
+        <v>0.062</v>
       </c>
       <c r="L16" s="7">
-        <v>1812.5</v>
+        <v>1875.0</v>
       </c>
       <c r="M16" s="1">
         <v>4500.0</v>
@@ -1497,7 +1497,7 @@
         <f t="shared" si="1"/>
         <v>0.03125</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="8">
         <f t="shared" si="2"/>
         <v>0.0625</v>
       </c>
@@ -1506,10 +1506,10 @@
         <v>1875</v>
       </c>
       <c r="K17" s="7">
-        <v>0.062</v>
+        <v>0.031</v>
       </c>
       <c r="L17" s="7">
-        <v>1875.0</v>
+        <v>1937.5</v>
       </c>
       <c r="M17" s="1">
         <v>3000.0</v>
@@ -1543,7 +1543,7 @@
         <f t="shared" ref="H18:H129" si="5">H2</f>
         <v>0.5</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="8">
         <f t="shared" si="2"/>
         <v>0.03125</v>
       </c>
@@ -1551,11 +1551,11 @@
         <f>1000 + 1000/16*15</f>
         <v>1937.5</v>
       </c>
-      <c r="K18" s="7">
-        <v>0.031</v>
+      <c r="K18" s="6">
+        <v>0.0</v>
       </c>
       <c r="L18" s="7">
-        <v>1937.5</v>
+        <v>2000.0</v>
       </c>
       <c r="M18" s="1">
         <v>1500.0</v>
@@ -1594,12 +1594,6 @@
         <v>0.0</v>
       </c>
       <c r="J19" s="7">
-        <v>2000.0</v>
-      </c>
-      <c r="K19" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="L19" s="7">
         <v>2000.0</v>
       </c>
       <c r="M19" s="1">

</xml_diff>